<commit_message>
working in risk calculator, processing deforestation files
</commit_message>
<xml_diff>
--- a/data/risk_calculator/conf/conf.xlsx
+++ b/data/risk_calculator/conf/conf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIAT\Code\BID\dci_fauno\data\risk_calculator\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5684A318-5585-4083-9ECA-FBD6E518726C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4BCE6A3-1809-4AD5-AD46-8180052CE85F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{1C78BAB9-C1D0-4BED-B8F8-A0E7D44C97AE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>parameter</t>
   </si>
@@ -49,16 +49,36 @@
   </si>
   <si>
     <t>2010_2012,2012_2013,2013_2014,2014_2015,2015_2016</t>
+  </si>
+  <si>
+    <t>def_value</t>
+  </si>
+  <si>
+    <t>def_pixel_size</t>
+  </si>
+  <si>
+    <t>uint8</t>
+  </si>
+  <si>
+    <t>def_dtype</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -81,13 +101,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -400,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA190DB3-6DA2-4E10-A40A-B26D7899FA62}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -424,7 +447,7 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -444,8 +467,35 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>30.716988260000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{ED14CBBE-2D07-4DC4-812C-607EBA4E59DD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
working in deforestation in risk calculator
</commit_message>
<xml_diff>
--- a/data/risk_calculator/conf/conf.xlsx
+++ b/data/risk_calculator/conf/conf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIAT\Code\BID\dci_fauno\data\risk_calculator\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4BCE6A3-1809-4AD5-AD46-8180052CE85F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A1059B-4673-4A09-A2A4-082C2C0BBBAD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{1C78BAB9-C1D0-4BED-B8F8-A0E7D44C97AE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>parameter</t>
   </si>
@@ -61,6 +61,18 @@
   </si>
   <si>
     <t>def_dtype</t>
+  </si>
+  <si>
+    <t>adm_url_source</t>
+  </si>
+  <si>
+    <t>https://geoportal.dane.gov.co/descargas/veredas/CRVeredas_2017.zip</t>
+  </si>
+  <si>
+    <t>plot_character_file</t>
+  </si>
+  <si>
+    <t>;</t>
   </si>
 </sst>
 </file>
@@ -423,7 +435,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA190DB3-6DA2-4E10-A40A-B26D7899FA62}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -491,11 +503,28 @@
         <v>10</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{ED14CBBE-2D07-4DC4-812C-607EBA4E59DD}"/>
+    <hyperlink ref="B8" r:id="rId2" xr:uid="{6E94A3A1-8DE8-452C-B096-B7E0C50B80AE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed deforestation compiling process
</commit_message>
<xml_diff>
--- a/data/risk_calculator/conf/conf.xlsx
+++ b/data/risk_calculator/conf/conf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIAT\Code\BID\dci_fauno\data\risk_calculator\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A1059B-4673-4A09-A2A4-082C2C0BBBAD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F14973-6CC1-4FB5-9B21-CFB106784E55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{1C78BAB9-C1D0-4BED-B8F8-A0E7D44C97AE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>parameter</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>;</t>
+  </si>
+  <si>
+    <t>glo_crs</t>
   </si>
 </sst>
 </file>
@@ -435,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA190DB3-6DA2-4E10-A40A-B26D7899FA62}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -457,72 +460,80 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>3116</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>30.716988260000001</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>30.716988260000001</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{ED14CBBE-2D07-4DC4-812C-607EBA4E59DD}"/>
-    <hyperlink ref="B8" r:id="rId2" xr:uid="{6E94A3A1-8DE8-452C-B096-B7E0C50B80AE}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{ED14CBBE-2D07-4DC4-812C-607EBA4E59DD}"/>
+    <hyperlink ref="B9" r:id="rId2" xr:uid="{6E94A3A1-8DE8-452C-B096-B7E0C50B80AE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
worked in the livestock module. it creates now a new layer with region and location for each plot
</commit_message>
<xml_diff>
--- a/data/risk_calculator/conf/conf.xlsx
+++ b/data/risk_calculator/conf/conf.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIAT\Code\BID\dci_fauno\data\risk_calculator\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F14973-6CC1-4FB5-9B21-CFB106784E55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6E89E3-76A7-41DE-9D5F-197336D5C94F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{1C78BAB9-C1D0-4BED-B8F8-A0E7D44C97AE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{1C78BAB9-C1D0-4BED-B8F8-A0E7D44C97AE}"/>
   </bookViews>
   <sheets>
     <sheet name="conf" sheetId="1" r:id="rId1"/>
+    <sheet name="buffer" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>parameter</t>
   </si>
@@ -69,20 +70,134 @@
     <t>https://geoportal.dane.gov.co/descargas/veredas/CRVeredas_2017.zip</t>
   </si>
   <si>
-    <t>plot_character_file</t>
-  </si>
-  <si>
     <t>;</t>
   </si>
   <si>
     <t>glo_crs</t>
+  </si>
+  <si>
+    <t>plo_character_file</t>
+  </si>
+  <si>
+    <t>codigosit</t>
+  </si>
+  <si>
+    <t>latitud</t>
+  </si>
+  <si>
+    <t>plo_src_ext_id</t>
+  </si>
+  <si>
+    <t>plo_src_lat</t>
+  </si>
+  <si>
+    <t>plo_src_lon</t>
+  </si>
+  <si>
+    <t>longitud</t>
+  </si>
+  <si>
+    <t>plo_src_adm1</t>
+  </si>
+  <si>
+    <t>plo_src_adm2</t>
+  </si>
+  <si>
+    <t>plo_src_adm3</t>
+  </si>
+  <si>
+    <t>departamento</t>
+  </si>
+  <si>
+    <t>municipio</t>
+  </si>
+  <si>
+    <t>vereda</t>
+  </si>
+  <si>
+    <t>plo_src_animals</t>
+  </si>
+  <si>
+    <t>totalanimales</t>
+  </si>
+  <si>
+    <t>plo_src_crs</t>
+  </si>
+  <si>
+    <t>adm_src_area</t>
+  </si>
+  <si>
+    <t>NOMB_MPIO</t>
+  </si>
+  <si>
+    <t>DPTOMPIO</t>
+  </si>
+  <si>
+    <t>NOMBRE_VER</t>
+  </si>
+  <si>
+    <t>CODIGO_VER</t>
+  </si>
+  <si>
+    <t>AREA_HA</t>
+  </si>
+  <si>
+    <t>adm_src_geometry</t>
+  </si>
+  <si>
+    <t>geometry</t>
+  </si>
+  <si>
+    <t>adm_src_adm1_name</t>
+  </si>
+  <si>
+    <t>adm_src_adm1_id</t>
+  </si>
+  <si>
+    <t>adm_src_adm3_name</t>
+  </si>
+  <si>
+    <t>adm_src_adm3_id</t>
+  </si>
+  <si>
+    <t>adm_src_adm2_name</t>
+  </si>
+  <si>
+    <t>adm_src_adm2_id</t>
+  </si>
+  <si>
+    <t>NOM_DEP</t>
+  </si>
+  <si>
+    <t>COD_DPTO</t>
+  </si>
+  <si>
+    <t>plo_lim_lat_low</t>
+  </si>
+  <si>
+    <t>plo_lim_lon_low</t>
+  </si>
+  <si>
+    <t>plo_lim_lat_upp</t>
+  </si>
+  <si>
+    <t>plo_lim_lon_upp</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>field_capacity</t>
+  </si>
+  <si>
+    <t>region_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,6 +209,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -120,9 +241,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -438,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA190DB3-6DA2-4E10-A40A-B26D7899FA62}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -460,7 +582,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>3116</v>
@@ -524,10 +646,170 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
-        <v>15</v>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26">
+        <v>4326</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27">
+        <v>-4.3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28">
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29">
+        <v>-79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30">
+        <v>-66</v>
       </c>
     </row>
   </sheetData>
@@ -538,4 +820,35 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0117B370-304C-4AF9-85F9-08AA565B4E3A}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added livesotck fixing data, also transformed raster to shp in deforestation module
</commit_message>
<xml_diff>
--- a/data/risk_calculator/conf/conf.xlsx
+++ b/data/risk_calculator/conf/conf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIAT\Code\BID\dci_fauno\data\risk_calculator\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6E89E3-76A7-41DE-9D5F-197336D5C94F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1E9053-EC5B-4AD5-AE5E-47A73C4DAE58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{1C78BAB9-C1D0-4BED-B8F8-A0E7D44C97AE}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>parameter</t>
   </si>
@@ -191,6 +191,105 @@
   </si>
   <si>
     <t>region_id</t>
+  </si>
+  <si>
+    <t>ANTIOQUIA</t>
+  </si>
+  <si>
+    <t>ATLÁNTICO</t>
+  </si>
+  <si>
+    <t>BOGOTÁ, D.C.</t>
+  </si>
+  <si>
+    <t>BOLÍVAR</t>
+  </si>
+  <si>
+    <t>BOYACÁ</t>
+  </si>
+  <si>
+    <t>CALDAS</t>
+  </si>
+  <si>
+    <t>CAQUETÁ</t>
+  </si>
+  <si>
+    <t>CAUCA</t>
+  </si>
+  <si>
+    <t>CESAR</t>
+  </si>
+  <si>
+    <t>CÓRDOBA</t>
+  </si>
+  <si>
+    <t>CUNDINAMARCA</t>
+  </si>
+  <si>
+    <t>CHOCÓ</t>
+  </si>
+  <si>
+    <t>HUILA</t>
+  </si>
+  <si>
+    <t>LA GUAJIRA</t>
+  </si>
+  <si>
+    <t>MAGDALENA</t>
+  </si>
+  <si>
+    <t>META</t>
+  </si>
+  <si>
+    <t>NARIÑO</t>
+  </si>
+  <si>
+    <t>NORTE DE SANTANDER</t>
+  </si>
+  <si>
+    <t>QUINDIO</t>
+  </si>
+  <si>
+    <t>RISARALDA</t>
+  </si>
+  <si>
+    <t>SANTANDER</t>
+  </si>
+  <si>
+    <t>SUCRE</t>
+  </si>
+  <si>
+    <t>TOLIMA</t>
+  </si>
+  <si>
+    <t>VALLE DEL CAUCA</t>
+  </si>
+  <si>
+    <t>ARAUCA</t>
+  </si>
+  <si>
+    <t>CASANARE</t>
+  </si>
+  <si>
+    <t>PUTUMAYO</t>
+  </si>
+  <si>
+    <t>ARCHIPIÉLAGO DE SAN ANDRÉS, PROVIDENCIA Y SANTA CATALINA</t>
+  </si>
+  <si>
+    <t>AMAZONAS</t>
+  </si>
+  <si>
+    <t>GUAINÍA</t>
+  </si>
+  <si>
+    <t>GUAVIARE</t>
+  </si>
+  <si>
+    <t>VAUPÉS</t>
+  </si>
+  <si>
+    <t>VICHADA</t>
   </si>
 </sst>
 </file>
@@ -824,10 +923,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0117B370-304C-4AF9-85F9-08AA565B4E3A}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -848,6 +947,369 @@
         <v>53</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>50</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>52</v>
+      </c>
+      <c r="B18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>63</v>
+      </c>
+      <c r="B20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>66</v>
+      </c>
+      <c r="B21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>68</v>
+      </c>
+      <c r="B22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>70</v>
+      </c>
+      <c r="B23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>73</v>
+      </c>
+      <c r="B24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>76</v>
+      </c>
+      <c r="B25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>81</v>
+      </c>
+      <c r="B26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>85</v>
+      </c>
+      <c r="B27" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>86</v>
+      </c>
+      <c r="B28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>88</v>
+      </c>
+      <c r="B29" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>91</v>
+      </c>
+      <c r="B30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>94</v>
+      </c>
+      <c r="B31" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>95</v>
+      </c>
+      <c r="B32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>97</v>
+      </c>
+      <c r="B33" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>99</v>
+      </c>
+      <c r="B34" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34">
+        <v>1.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
working in risk calculator
</commit_message>
<xml_diff>
--- a/data/risk_calculator/conf/conf.xlsx
+++ b/data/risk_calculator/conf/conf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIAT\Code\BID\dci_fauno\data\risk_calculator\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1E9053-EC5B-4AD5-AE5E-47A73C4DAE58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F388E0CB-6CC3-487D-8DA5-BA9FDF62D3EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{1C78BAB9-C1D0-4BED-B8F8-A0E7D44C97AE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{1C78BAB9-C1D0-4BED-B8F8-A0E7D44C97AE}"/>
   </bookViews>
   <sheets>
     <sheet name="conf" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>parameter</t>
   </si>
@@ -290,6 +290,18 @@
   </si>
   <si>
     <t>VICHADA</t>
+  </si>
+  <si>
+    <t>ris_years</t>
+  </si>
+  <si>
+    <t>ris_types_analysis</t>
+  </si>
+  <si>
+    <t>detail,summary</t>
+  </si>
+  <si>
+    <t>2010, 2012, 2019</t>
   </si>
 </sst>
 </file>
@@ -340,10 +352,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -659,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA190DB3-6DA2-4E10-A40A-B26D7899FA62}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:A30"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -799,7 +813,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -807,7 +821,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -815,7 +829,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -823,7 +837,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -831,7 +845,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -839,7 +853,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -847,7 +861,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -855,7 +869,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -863,7 +877,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -871,7 +885,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -879,7 +893,7 @@
         <v>4326</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -887,7 +901,7 @@
         <v>-4.3</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>50</v>
       </c>
@@ -895,7 +909,7 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>49</v>
       </c>
@@ -903,12 +917,31 @@
         <v>-79</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>51</v>
       </c>
       <c r="B30">
         <v>-66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="4">
+        <v>2019</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -925,7 +958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0117B370-304C-4AF9-85F9-08AA565B4E3A}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>